<commit_message>
add possibility some numbers and strings sort; add test for it
</commit_message>
<xml_diff>
--- a/6/2020.01.26_Exported_Session_5_results_ITI.xlsx
+++ b/6/2020.01.26_Exported_Session_5_results_ITI.xlsx
@@ -32,22 +32,22 @@
     <t>Igor</t>
   </si>
   <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>Olga</t>
+  </si>
+  <si>
     <t>OOP</t>
   </si>
   <si>
-    <t>NN</t>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>Vania</t>
   </si>
   <si>
     <t>java</t>
-  </si>
-  <si>
-    <t>DV</t>
-  </si>
-  <si>
-    <t>Vania</t>
-  </si>
-  <si>
-    <t>Olga</t>
   </si>
 </sst>
 </file>
@@ -130,7 +130,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -138,10 +138,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="0">
         <v>8</v>
@@ -158,7 +158,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -183,7 +183,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" s="0">
         <v>9</v>
@@ -197,7 +197,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="0">
         <v>9</v>
@@ -208,13 +208,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -222,13 +222,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -236,13 +236,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="D10" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -250,13 +250,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="D11" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -264,10 +264,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0">
         <v>10</v>
@@ -278,13 +278,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="D13" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>